<commit_message>
add gender column to participants list
</commit_message>
<xml_diff>
--- a/data/arg2 participants.xlsx
+++ b/data/arg2 participants.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="43">
   <si>
     <t>subject</t>
   </si>
@@ -139,6 +139,15 @@
   </si>
   <si>
     <t>TRUE</t>
+  </si>
+  <si>
+    <t>m</t>
+  </si>
+  <si>
+    <t>f</t>
+  </si>
+  <si>
+    <t>gender</t>
   </si>
 </sst>
 </file>
@@ -639,21 +648,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G28"/>
+  <dimension ref="A1:H28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="3" width="10.69921875" customWidth="1"/>
-    <col min="4" max="4" width="10.3984375" customWidth="1"/>
-    <col min="5" max="6" width="10.69921875" customWidth="1"/>
-    <col min="7" max="7" width="36.09765625" customWidth="1"/>
+    <col min="1" max="4" width="10.69921875" customWidth="1"/>
+    <col min="5" max="5" width="10.3984375" customWidth="1"/>
+    <col min="6" max="7" width="10.69921875" customWidth="1"/>
+    <col min="8" max="8" width="36.09765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -661,489 +670,573 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
         <v>6</v>
       </c>
-      <c r="C2">
+      <c r="C2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D2">
         <v>20111106</v>
       </c>
-      <c r="D2">
+      <c r="E2">
         <v>20191220</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
         <v>8</v>
       </c>
-      <c r="C3">
+      <c r="C3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D3">
         <v>20131024</v>
       </c>
-      <c r="D3">
+      <c r="E3">
         <v>20191220</v>
       </c>
-      <c r="E3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
         <v>10</v>
       </c>
-      <c r="C4">
+      <c r="C4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D4">
         <v>20131130</v>
       </c>
-      <c r="D4">
+      <c r="E4">
         <v>20191220</v>
       </c>
-      <c r="E4" t="s">
-        <v>9</v>
-      </c>
       <c r="F4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G4" t="s">
         <v>39</v>
       </c>
-      <c r="G4" t="s">
+      <c r="H4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
         <v>12</v>
       </c>
-      <c r="C5">
+      <c r="C5" t="s">
+        <v>40</v>
+      </c>
+      <c r="D5">
         <v>20131022</v>
       </c>
-      <c r="D5">
+      <c r="E5">
         <v>20191220</v>
       </c>
-      <c r="E5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
         <v>13</v>
       </c>
-      <c r="C6">
+      <c r="C6" t="s">
+        <v>41</v>
+      </c>
+      <c r="D6">
         <v>20140623</v>
       </c>
-      <c r="D6">
+      <c r="E6">
         <v>20191220</v>
       </c>
-      <c r="E6" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
         <v>14</v>
       </c>
-      <c r="C7">
+      <c r="C7" t="s">
+        <v>40</v>
+      </c>
+      <c r="D7">
         <v>20140109</v>
       </c>
-      <c r="D7">
+      <c r="E7">
         <v>20191220</v>
       </c>
-      <c r="E7" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
         <v>15</v>
       </c>
-      <c r="C8">
+      <c r="C8" t="s">
+        <v>40</v>
+      </c>
+      <c r="D8">
         <v>20130814</v>
       </c>
-      <c r="D8">
+      <c r="E8">
         <v>20191222</v>
       </c>
-      <c r="E8" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" t="s">
         <v>16</v>
       </c>
-      <c r="C9">
+      <c r="C9" t="s">
+        <v>41</v>
+      </c>
+      <c r="D9">
         <v>20130531</v>
       </c>
-      <c r="D9">
+      <c r="E9">
         <v>20191222</v>
       </c>
-      <c r="E9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" t="s">
         <v>17</v>
       </c>
-      <c r="C10">
+      <c r="C10" t="s">
+        <v>41</v>
+      </c>
+      <c r="D10">
         <v>20140523</v>
       </c>
-      <c r="D10">
+      <c r="E10">
         <v>20191222</v>
       </c>
-      <c r="E10" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11" t="s">
         <v>18</v>
       </c>
-      <c r="C11">
+      <c r="C11" t="s">
+        <v>40</v>
+      </c>
+      <c r="D11">
         <v>20140112</v>
       </c>
-      <c r="D11">
+      <c r="E11">
         <v>20191222</v>
       </c>
-      <c r="E11" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F11" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12" t="s">
         <v>19</v>
       </c>
-      <c r="C12">
+      <c r="C12" t="s">
+        <v>41</v>
+      </c>
+      <c r="D12">
         <v>20110221</v>
       </c>
-      <c r="D12">
+      <c r="E12">
         <v>20191222</v>
       </c>
-      <c r="E12" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F12" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="B13" t="s">
         <v>20</v>
       </c>
-      <c r="C13">
+      <c r="C13" t="s">
+        <v>40</v>
+      </c>
+      <c r="D13">
         <v>20130626</v>
       </c>
-      <c r="D13">
+      <c r="E13">
         <v>20191222</v>
       </c>
-      <c r="E13" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F13" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
       <c r="B14" t="s">
         <v>21</v>
       </c>
-      <c r="C14">
+      <c r="C14" t="s">
+        <v>40</v>
+      </c>
+      <c r="D14">
         <v>20120626</v>
       </c>
-      <c r="D14">
+      <c r="E14">
         <v>20191222</v>
       </c>
-      <c r="E14" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F14" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
       <c r="B15" t="s">
         <v>22</v>
       </c>
-      <c r="C15">
+      <c r="C15" t="s">
+        <v>40</v>
+      </c>
+      <c r="D15">
         <v>20100628</v>
       </c>
-      <c r="D15">
+      <c r="E15">
         <v>20191222</v>
       </c>
-      <c r="E15" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F15" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
       <c r="B16" t="s">
         <v>23</v>
       </c>
-      <c r="C16">
+      <c r="C16" t="s">
+        <v>40</v>
+      </c>
+      <c r="D16">
         <v>20130924</v>
       </c>
-      <c r="D16">
+      <c r="E16">
         <v>20191222</v>
       </c>
-      <c r="E16" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F16" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
       <c r="B17" t="s">
         <v>24</v>
       </c>
-      <c r="C17">
+      <c r="C17" t="s">
+        <v>40</v>
+      </c>
+      <c r="D17">
         <v>20151221</v>
       </c>
-      <c r="D17">
+      <c r="E17">
         <v>20191222</v>
       </c>
-      <c r="E17" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F17" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
       <c r="B18" t="s">
         <v>25</v>
       </c>
-      <c r="C18">
+      <c r="C18" t="s">
+        <v>40</v>
+      </c>
+      <c r="D18">
         <v>20140620</v>
       </c>
-      <c r="D18">
+      <c r="E18">
         <v>20191222</v>
       </c>
-      <c r="E18" t="s">
-        <v>9</v>
-      </c>
-      <c r="G18" t="s">
+      <c r="F18" t="s">
+        <v>9</v>
+      </c>
+      <c r="H18" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
       <c r="B19" t="s">
         <v>27</v>
       </c>
-      <c r="C19">
+      <c r="C19" t="s">
+        <v>40</v>
+      </c>
+      <c r="D19">
         <v>20110416</v>
       </c>
-      <c r="D19">
+      <c r="E19">
         <v>20200102</v>
       </c>
-      <c r="E19" t="s">
+      <c r="F19" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
       <c r="B20" t="s">
         <v>28</v>
       </c>
-      <c r="C20">
+      <c r="C20" t="s">
+        <v>41</v>
+      </c>
+      <c r="D20">
         <v>20130622</v>
       </c>
-      <c r="D20">
+      <c r="E20">
         <v>20200102</v>
       </c>
-      <c r="E20" t="s">
+      <c r="F20" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
       <c r="B21" t="s">
         <v>29</v>
       </c>
-      <c r="C21">
+      <c r="C21" t="s">
+        <v>41</v>
+      </c>
+      <c r="D21">
         <v>20160419</v>
       </c>
-      <c r="D21">
+      <c r="E21">
         <v>20200102</v>
       </c>
-      <c r="E21" t="s">
+      <c r="F21" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
       <c r="B22" t="s">
         <v>30</v>
       </c>
-      <c r="C22">
+      <c r="C22" t="s">
+        <v>40</v>
+      </c>
+      <c r="D22">
         <v>20100409</v>
       </c>
-      <c r="D22">
+      <c r="E22">
         <v>20200102</v>
       </c>
-      <c r="E22" t="s">
+      <c r="F22" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
       <c r="B23" t="s">
         <v>31</v>
       </c>
-      <c r="C23">
+      <c r="C23" t="s">
+        <v>40</v>
+      </c>
+      <c r="D23">
         <v>20130305</v>
       </c>
-      <c r="D23">
+      <c r="E23">
         <v>20200102</v>
       </c>
-      <c r="E23" t="s">
+      <c r="F23" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
       <c r="B24" t="s">
         <v>32</v>
       </c>
-      <c r="C24">
+      <c r="C24" t="s">
+        <v>41</v>
+      </c>
+      <c r="D24">
         <v>20100729</v>
       </c>
-      <c r="D24">
+      <c r="E24">
         <v>20200102</v>
       </c>
-      <c r="E24" t="s">
+      <c r="F24" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
       <c r="B25" t="s">
         <v>33</v>
       </c>
-      <c r="C25">
+      <c r="C25" t="s">
+        <v>40</v>
+      </c>
+      <c r="D25">
         <v>20150611</v>
       </c>
-      <c r="D25">
+      <c r="E25">
         <v>20200102</v>
       </c>
-      <c r="E25" t="s">
+      <c r="F25" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
       <c r="B26" t="s">
         <v>34</v>
       </c>
-      <c r="C26">
+      <c r="C26" t="s">
+        <v>40</v>
+      </c>
+      <c r="D26">
         <v>20150512</v>
       </c>
-      <c r="D26">
+      <c r="E26">
         <v>20200102</v>
       </c>
-      <c r="E26" t="s">
+      <c r="F26" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
       <c r="B27" t="s">
         <v>35</v>
       </c>
-      <c r="C27">
+      <c r="C27" t="s">
+        <v>41</v>
+      </c>
+      <c r="D27">
         <v>20140911</v>
       </c>
-      <c r="D27">
+      <c r="E27">
         <v>20200102</v>
       </c>
-      <c r="E27" t="s">
+      <c r="F27" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
       <c r="B28" t="s">
         <v>36</v>
       </c>
-      <c r="C28">
+      <c r="C28" t="s">
+        <v>41</v>
+      </c>
+      <c r="D28">
         <v>20140204</v>
       </c>
-      <c r="D28">
+      <c r="E28">
         <v>20200102</v>
       </c>
-      <c r="E28" t="s">
+      <c r="F28" t="s">
         <v>7</v>
       </c>
-      <c r="G28" t="s">
+      <c r="H28" t="s">
         <v>37</v>
       </c>
     </row>

</xml_diff>